<commit_message>
check update print Congratulations
</commit_message>
<xml_diff>
--- a/studentData.xlsx
+++ b/studentData.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11295" windowWidth="21600" xWindow="1230" yWindow="2280"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1230" yWindow="2280" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -43,18 +43,86 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -367,7 +435,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="2" min="1" width="13.5703125"/>
+    <col width="13.5703125" customWidth="1" min="1" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -417,10 +485,10 @@
         <v>1945</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>